<commit_message>
using tetraminoes movements in tests
</commit_message>
<xml_diff>
--- a/tetris.xlsx
+++ b/tetris.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="30840" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14840" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="board" sheetId="1" r:id="rId1"/>
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -927,7 +927,7 @@
     <row r="2" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="12"/>
@@ -985,7 +985,7 @@
     <row r="3" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="15"/>
@@ -1043,7 +1043,7 @@
     <row r="4" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
@@ -1101,7 +1101,7 @@
     <row r="5" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="2"/>
@@ -1159,7 +1159,7 @@
     <row r="6" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="2"/>
@@ -1217,7 +1217,7 @@
     <row r="7" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="2"/>
@@ -1275,7 +1275,7 @@
     <row r="8" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="2"/>
@@ -1333,7 +1333,7 @@
     <row r="9" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="2"/>
@@ -1391,7 +1391,7 @@
     <row r="10" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="2"/>
@@ -1449,7 +1449,7 @@
     <row r="11" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="2"/>
@@ -1565,7 +1565,7 @@
     <row r="13" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="2"/>
@@ -1623,7 +1623,7 @@
     <row r="14" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="2"/>
@@ -1681,7 +1681,7 @@
     <row r="15" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="2"/>
@@ -1739,7 +1739,7 @@
     <row r="16" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="2"/>
@@ -1797,7 +1797,7 @@
     <row r="17" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="2"/>
@@ -1855,7 +1855,7 @@
     <row r="18" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="2"/>
@@ -1913,7 +1913,7 @@
     <row r="19" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="2"/>
@@ -1971,7 +1971,7 @@
     <row r="20" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="2"/>
@@ -2031,7 +2031,7 @@
     <row r="21" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="2"/>
@@ -2089,7 +2089,7 @@
     <row r="22" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="2"/>
@@ -2149,7 +2149,7 @@
     <row r="23" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
@@ -2208,34 +2208,34 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G24" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H24" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I24" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J24" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K24" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L24" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -5425,8 +5425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48:L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5511,8 +5511,8 @@
     </row>
     <row r="2" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="45"/>
-      <c r="B2" s="45">
-        <v>21</v>
+      <c r="B2" s="1">
+        <v>1</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="20"/>
@@ -5525,8 +5525,8 @@
       <c r="K2" s="20"/>
       <c r="L2" s="21"/>
       <c r="M2" s="45"/>
-      <c r="N2" s="45">
-        <v>21</v>
+      <c r="N2" s="1">
+        <v>1</v>
       </c>
       <c r="O2" s="19"/>
       <c r="P2" s="20"/>
@@ -5541,8 +5541,8 @@
       <c r="W2" s="20"/>
       <c r="X2" s="21"/>
       <c r="Y2" s="45"/>
-      <c r="Z2" s="45">
-        <v>21</v>
+      <c r="Z2" s="1">
+        <v>1</v>
       </c>
       <c r="AA2" s="19"/>
       <c r="AB2" s="20"/>
@@ -5557,8 +5557,8 @@
       <c r="AI2" s="20"/>
       <c r="AJ2" s="21"/>
       <c r="AK2" s="45"/>
-      <c r="AL2" s="45">
-        <v>21</v>
+      <c r="AL2" s="1">
+        <v>1</v>
       </c>
       <c r="AM2" s="19"/>
       <c r="AN2" s="20"/>
@@ -5602,8 +5602,8 @@
     </row>
     <row r="3" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="45"/>
-      <c r="B3" s="45">
-        <v>20</v>
+      <c r="B3" s="1">
+        <v>2</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="23"/>
@@ -5624,8 +5624,8 @@
       <c r="K3" s="23"/>
       <c r="L3" s="25"/>
       <c r="M3" s="45"/>
-      <c r="N3" s="45">
-        <v>20</v>
+      <c r="N3" s="1">
+        <v>2</v>
       </c>
       <c r="O3" s="22"/>
       <c r="P3" s="23"/>
@@ -5644,8 +5644,8 @@
       <c r="W3" s="23"/>
       <c r="X3" s="25"/>
       <c r="Y3" s="45"/>
-      <c r="Z3" s="45">
-        <v>20</v>
+      <c r="Z3" s="1">
+        <v>2</v>
       </c>
       <c r="AA3" s="22"/>
       <c r="AB3" s="23"/>
@@ -5664,8 +5664,8 @@
       <c r="AI3" s="23"/>
       <c r="AJ3" s="25"/>
       <c r="AK3" s="45"/>
-      <c r="AL3" s="45">
-        <v>20</v>
+      <c r="AL3" s="1">
+        <v>2</v>
       </c>
       <c r="AM3" s="22"/>
       <c r="AN3" s="23"/>
@@ -5709,8 +5709,8 @@
     </row>
     <row r="4" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="45"/>
-      <c r="B4" s="45">
-        <v>19</v>
+      <c r="B4" s="1">
+        <v>3</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="27"/>
@@ -5723,8 +5723,8 @@
       <c r="K4" s="27"/>
       <c r="L4" s="28"/>
       <c r="M4" s="45"/>
-      <c r="N4" s="45">
-        <v>19</v>
+      <c r="N4" s="1">
+        <v>3</v>
       </c>
       <c r="O4" s="26"/>
       <c r="P4" s="27"/>
@@ -5737,8 +5737,8 @@
       <c r="W4" s="27"/>
       <c r="X4" s="28"/>
       <c r="Y4" s="45"/>
-      <c r="Z4" s="45">
-        <v>19</v>
+      <c r="Z4" s="1">
+        <v>3</v>
       </c>
       <c r="AA4" s="26"/>
       <c r="AB4" s="27"/>
@@ -5751,8 +5751,8 @@
       <c r="AI4" s="27"/>
       <c r="AJ4" s="28"/>
       <c r="AK4" s="45"/>
-      <c r="AL4" s="45">
-        <v>19</v>
+      <c r="AL4" s="1">
+        <v>3</v>
       </c>
       <c r="AM4" s="26"/>
       <c r="AN4" s="27"/>
@@ -5792,8 +5792,8 @@
     </row>
     <row r="5" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="45"/>
-      <c r="B5" s="45">
-        <v>18</v>
+      <c r="B5" s="1">
+        <v>4</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="30"/>
@@ -5806,8 +5806,8 @@
       <c r="K5" s="30"/>
       <c r="L5" s="31"/>
       <c r="M5" s="45"/>
-      <c r="N5" s="45">
-        <v>18</v>
+      <c r="N5" s="1">
+        <v>4</v>
       </c>
       <c r="O5" s="29"/>
       <c r="P5" s="30"/>
@@ -5820,8 +5820,8 @@
       <c r="W5" s="30"/>
       <c r="X5" s="31"/>
       <c r="Y5" s="45"/>
-      <c r="Z5" s="45">
-        <v>18</v>
+      <c r="Z5" s="1">
+        <v>4</v>
       </c>
       <c r="AA5" s="29"/>
       <c r="AB5" s="30"/>
@@ -5834,8 +5834,8 @@
       <c r="AI5" s="30"/>
       <c r="AJ5" s="31"/>
       <c r="AK5" s="45"/>
-      <c r="AL5" s="45">
-        <v>18</v>
+      <c r="AL5" s="1">
+        <v>4</v>
       </c>
       <c r="AM5" s="29"/>
       <c r="AN5" s="30"/>
@@ -5875,8 +5875,8 @@
     </row>
     <row r="6" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="45"/>
-      <c r="B6" s="45">
-        <v>17</v>
+      <c r="B6" s="1">
+        <v>5</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="30"/>
@@ -5889,8 +5889,8 @@
       <c r="K6" s="30"/>
       <c r="L6" s="31"/>
       <c r="M6" s="45"/>
-      <c r="N6" s="45">
-        <v>17</v>
+      <c r="N6" s="1">
+        <v>5</v>
       </c>
       <c r="O6" s="29"/>
       <c r="P6" s="30"/>
@@ -5903,8 +5903,8 @@
       <c r="W6" s="30"/>
       <c r="X6" s="31"/>
       <c r="Y6" s="45"/>
-      <c r="Z6" s="45">
-        <v>17</v>
+      <c r="Z6" s="1">
+        <v>5</v>
       </c>
       <c r="AA6" s="29"/>
       <c r="AB6" s="30"/>
@@ -5917,8 +5917,8 @@
       <c r="AI6" s="30"/>
       <c r="AJ6" s="31"/>
       <c r="AK6" s="45"/>
-      <c r="AL6" s="45">
-        <v>17</v>
+      <c r="AL6" s="1">
+        <v>5</v>
       </c>
       <c r="AM6" s="29"/>
       <c r="AN6" s="30"/>
@@ -5958,8 +5958,8 @@
     </row>
     <row r="7" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="45"/>
-      <c r="B7" s="45">
-        <v>16</v>
+      <c r="B7" s="1">
+        <v>6</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="30"/>
@@ -5972,8 +5972,8 @@
       <c r="K7" s="30"/>
       <c r="L7" s="31"/>
       <c r="M7" s="45"/>
-      <c r="N7" s="45">
-        <v>16</v>
+      <c r="N7" s="1">
+        <v>6</v>
       </c>
       <c r="O7" s="29"/>
       <c r="P7" s="30"/>
@@ -5986,8 +5986,8 @@
       <c r="W7" s="30"/>
       <c r="X7" s="31"/>
       <c r="Y7" s="45"/>
-      <c r="Z7" s="45">
-        <v>16</v>
+      <c r="Z7" s="1">
+        <v>6</v>
       </c>
       <c r="AA7" s="29"/>
       <c r="AB7" s="30"/>
@@ -6000,8 +6000,8 @@
       <c r="AI7" s="30"/>
       <c r="AJ7" s="31"/>
       <c r="AK7" s="45"/>
-      <c r="AL7" s="45">
-        <v>16</v>
+      <c r="AL7" s="1">
+        <v>6</v>
       </c>
       <c r="AM7" s="29"/>
       <c r="AN7" s="30"/>
@@ -6041,8 +6041,8 @@
     </row>
     <row r="8" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="45"/>
-      <c r="B8" s="45">
-        <v>15</v>
+      <c r="B8" s="1">
+        <v>7</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="30"/>
@@ -6055,8 +6055,8 @@
       <c r="K8" s="30"/>
       <c r="L8" s="31"/>
       <c r="M8" s="45"/>
-      <c r="N8" s="45">
-        <v>15</v>
+      <c r="N8" s="1">
+        <v>7</v>
       </c>
       <c r="O8" s="29"/>
       <c r="P8" s="30"/>
@@ -6069,8 +6069,8 @@
       <c r="W8" s="30"/>
       <c r="X8" s="31"/>
       <c r="Y8" s="45"/>
-      <c r="Z8" s="45">
-        <v>15</v>
+      <c r="Z8" s="1">
+        <v>7</v>
       </c>
       <c r="AA8" s="29"/>
       <c r="AB8" s="30"/>
@@ -6083,8 +6083,8 @@
       <c r="AI8" s="30"/>
       <c r="AJ8" s="31"/>
       <c r="AK8" s="45"/>
-      <c r="AL8" s="45">
-        <v>15</v>
+      <c r="AL8" s="1">
+        <v>7</v>
       </c>
       <c r="AM8" s="29"/>
       <c r="AN8" s="30"/>
@@ -6124,8 +6124,8 @@
     </row>
     <row r="9" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="45"/>
-      <c r="B9" s="45">
-        <v>14</v>
+      <c r="B9" s="1">
+        <v>8</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="30"/>
@@ -6138,8 +6138,8 @@
       <c r="K9" s="30"/>
       <c r="L9" s="31"/>
       <c r="M9" s="45"/>
-      <c r="N9" s="45">
-        <v>14</v>
+      <c r="N9" s="1">
+        <v>8</v>
       </c>
       <c r="O9" s="29"/>
       <c r="P9" s="30"/>
@@ -6152,8 +6152,8 @@
       <c r="W9" s="30"/>
       <c r="X9" s="31"/>
       <c r="Y9" s="45"/>
-      <c r="Z9" s="45">
-        <v>14</v>
+      <c r="Z9" s="1">
+        <v>8</v>
       </c>
       <c r="AA9" s="29"/>
       <c r="AB9" s="30"/>
@@ -6166,8 +6166,8 @@
       <c r="AI9" s="30"/>
       <c r="AJ9" s="31"/>
       <c r="AK9" s="45"/>
-      <c r="AL9" s="45">
-        <v>14</v>
+      <c r="AL9" s="1">
+        <v>8</v>
       </c>
       <c r="AM9" s="29"/>
       <c r="AN9" s="30"/>
@@ -6207,8 +6207,8 @@
     </row>
     <row r="10" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="45"/>
-      <c r="B10" s="45">
-        <v>13</v>
+      <c r="B10" s="1">
+        <v>9</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
@@ -6221,8 +6221,8 @@
       <c r="K10" s="30"/>
       <c r="L10" s="31"/>
       <c r="M10" s="45"/>
-      <c r="N10" s="45">
-        <v>13</v>
+      <c r="N10" s="1">
+        <v>9</v>
       </c>
       <c r="O10" s="29"/>
       <c r="P10" s="30"/>
@@ -6235,8 +6235,8 @@
       <c r="W10" s="30"/>
       <c r="X10" s="31"/>
       <c r="Y10" s="45"/>
-      <c r="Z10" s="45">
-        <v>13</v>
+      <c r="Z10" s="1">
+        <v>9</v>
       </c>
       <c r="AA10" s="29"/>
       <c r="AB10" s="30"/>
@@ -6249,8 +6249,8 @@
       <c r="AI10" s="30"/>
       <c r="AJ10" s="31"/>
       <c r="AK10" s="45"/>
-      <c r="AL10" s="45">
-        <v>13</v>
+      <c r="AL10" s="1">
+        <v>9</v>
       </c>
       <c r="AM10" s="29"/>
       <c r="AN10" s="30"/>
@@ -6290,8 +6290,8 @@
     </row>
     <row r="11" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="45"/>
-      <c r="B11" s="45">
-        <v>12</v>
+      <c r="B11" s="1">
+        <v>10</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="30"/>
@@ -6304,8 +6304,8 @@
       <c r="K11" s="30"/>
       <c r="L11" s="31"/>
       <c r="M11" s="45"/>
-      <c r="N11" s="45">
-        <v>12</v>
+      <c r="N11" s="1">
+        <v>10</v>
       </c>
       <c r="O11" s="29"/>
       <c r="P11" s="30"/>
@@ -6318,8 +6318,8 @@
       <c r="W11" s="30"/>
       <c r="X11" s="31"/>
       <c r="Y11" s="45"/>
-      <c r="Z11" s="45">
-        <v>12</v>
+      <c r="Z11" s="1">
+        <v>10</v>
       </c>
       <c r="AA11" s="29"/>
       <c r="AB11" s="30"/>
@@ -6332,8 +6332,8 @@
       <c r="AI11" s="30"/>
       <c r="AJ11" s="31"/>
       <c r="AK11" s="45"/>
-      <c r="AL11" s="45">
-        <v>12</v>
+      <c r="AL11" s="1">
+        <v>10</v>
       </c>
       <c r="AM11" s="29"/>
       <c r="AN11" s="30"/>
@@ -6373,7 +6373,7 @@
     </row>
     <row r="12" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="45"/>
-      <c r="B12" s="45">
+      <c r="B12" s="1">
         <v>11</v>
       </c>
       <c r="C12" s="29"/>
@@ -6387,7 +6387,7 @@
       <c r="K12" s="30"/>
       <c r="L12" s="31"/>
       <c r="M12" s="45"/>
-      <c r="N12" s="45">
+      <c r="N12" s="1">
         <v>11</v>
       </c>
       <c r="O12" s="29"/>
@@ -6401,7 +6401,7 @@
       <c r="W12" s="30"/>
       <c r="X12" s="31"/>
       <c r="Y12" s="45"/>
-      <c r="Z12" s="45">
+      <c r="Z12" s="1">
         <v>11</v>
       </c>
       <c r="AA12" s="29"/>
@@ -6415,7 +6415,7 @@
       <c r="AI12" s="30"/>
       <c r="AJ12" s="31"/>
       <c r="AK12" s="45"/>
-      <c r="AL12" s="45">
+      <c r="AL12" s="1">
         <v>11</v>
       </c>
       <c r="AM12" s="29"/>
@@ -6456,8 +6456,8 @@
     </row>
     <row r="13" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="45"/>
-      <c r="B13" s="45">
-        <v>10</v>
+      <c r="B13" s="1">
+        <v>12</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="30"/>
@@ -6470,8 +6470,8 @@
       <c r="K13" s="30"/>
       <c r="L13" s="31"/>
       <c r="M13" s="45"/>
-      <c r="N13" s="45">
-        <v>10</v>
+      <c r="N13" s="1">
+        <v>12</v>
       </c>
       <c r="O13" s="29"/>
       <c r="P13" s="30"/>
@@ -6484,8 +6484,8 @@
       <c r="W13" s="30"/>
       <c r="X13" s="31"/>
       <c r="Y13" s="45"/>
-      <c r="Z13" s="45">
-        <v>10</v>
+      <c r="Z13" s="1">
+        <v>12</v>
       </c>
       <c r="AA13" s="29"/>
       <c r="AB13" s="30"/>
@@ -6498,8 +6498,8 @@
       <c r="AI13" s="30"/>
       <c r="AJ13" s="31"/>
       <c r="AK13" s="45"/>
-      <c r="AL13" s="45">
-        <v>10</v>
+      <c r="AL13" s="1">
+        <v>12</v>
       </c>
       <c r="AM13" s="29"/>
       <c r="AN13" s="30"/>
@@ -6539,8 +6539,8 @@
     </row>
     <row r="14" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="45"/>
-      <c r="B14" s="45">
-        <v>9</v>
+      <c r="B14" s="1">
+        <v>13</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="30"/>
@@ -6553,8 +6553,8 @@
       <c r="K14" s="30"/>
       <c r="L14" s="31"/>
       <c r="M14" s="45"/>
-      <c r="N14" s="45">
-        <v>9</v>
+      <c r="N14" s="1">
+        <v>13</v>
       </c>
       <c r="O14" s="29"/>
       <c r="P14" s="30"/>
@@ -6567,8 +6567,8 @@
       <c r="W14" s="30"/>
       <c r="X14" s="31"/>
       <c r="Y14" s="45"/>
-      <c r="Z14" s="45">
-        <v>9</v>
+      <c r="Z14" s="1">
+        <v>13</v>
       </c>
       <c r="AA14" s="29"/>
       <c r="AB14" s="30"/>
@@ -6581,8 +6581,8 @@
       <c r="AI14" s="30"/>
       <c r="AJ14" s="31"/>
       <c r="AK14" s="45"/>
-      <c r="AL14" s="45">
-        <v>9</v>
+      <c r="AL14" s="1">
+        <v>13</v>
       </c>
       <c r="AM14" s="29"/>
       <c r="AN14" s="30"/>
@@ -6622,8 +6622,8 @@
     </row>
     <row r="15" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="45"/>
-      <c r="B15" s="45">
-        <v>8</v>
+      <c r="B15" s="1">
+        <v>14</v>
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="30"/>
@@ -6636,8 +6636,8 @@
       <c r="K15" s="30"/>
       <c r="L15" s="31"/>
       <c r="M15" s="45"/>
-      <c r="N15" s="45">
-        <v>8</v>
+      <c r="N15" s="1">
+        <v>14</v>
       </c>
       <c r="O15" s="29"/>
       <c r="P15" s="30"/>
@@ -6650,8 +6650,8 @@
       <c r="W15" s="30"/>
       <c r="X15" s="31"/>
       <c r="Y15" s="45"/>
-      <c r="Z15" s="45">
-        <v>8</v>
+      <c r="Z15" s="1">
+        <v>14</v>
       </c>
       <c r="AA15" s="29"/>
       <c r="AB15" s="30"/>
@@ -6664,8 +6664,8 @@
       <c r="AI15" s="30"/>
       <c r="AJ15" s="31"/>
       <c r="AK15" s="45"/>
-      <c r="AL15" s="45">
-        <v>8</v>
+      <c r="AL15" s="1">
+        <v>14</v>
       </c>
       <c r="AM15" s="29"/>
       <c r="AN15" s="30"/>
@@ -6705,8 +6705,8 @@
     </row>
     <row r="16" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="45"/>
-      <c r="B16" s="45">
-        <v>7</v>
+      <c r="B16" s="1">
+        <v>15</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16" s="30"/>
@@ -6719,8 +6719,8 @@
       <c r="K16" s="30"/>
       <c r="L16" s="31"/>
       <c r="M16" s="45"/>
-      <c r="N16" s="45">
-        <v>7</v>
+      <c r="N16" s="1">
+        <v>15</v>
       </c>
       <c r="O16" s="29"/>
       <c r="P16" s="30"/>
@@ -6733,8 +6733,8 @@
       <c r="W16" s="30"/>
       <c r="X16" s="31"/>
       <c r="Y16" s="45"/>
-      <c r="Z16" s="45">
-        <v>7</v>
+      <c r="Z16" s="1">
+        <v>15</v>
       </c>
       <c r="AA16" s="29"/>
       <c r="AB16" s="30"/>
@@ -6747,8 +6747,8 @@
       <c r="AI16" s="30"/>
       <c r="AJ16" s="31"/>
       <c r="AK16" s="45"/>
-      <c r="AL16" s="45">
-        <v>7</v>
+      <c r="AL16" s="1">
+        <v>15</v>
       </c>
       <c r="AM16" s="29"/>
       <c r="AN16" s="30"/>
@@ -6788,8 +6788,8 @@
     </row>
     <row r="17" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="45"/>
-      <c r="B17" s="45">
-        <v>6</v>
+      <c r="B17" s="1">
+        <v>16</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="30"/>
@@ -6802,8 +6802,8 @@
       <c r="K17" s="30"/>
       <c r="L17" s="31"/>
       <c r="M17" s="45"/>
-      <c r="N17" s="45">
-        <v>6</v>
+      <c r="N17" s="1">
+        <v>16</v>
       </c>
       <c r="O17" s="29"/>
       <c r="P17" s="30"/>
@@ -6816,8 +6816,8 @@
       <c r="W17" s="30"/>
       <c r="X17" s="31"/>
       <c r="Y17" s="45"/>
-      <c r="Z17" s="45">
-        <v>6</v>
+      <c r="Z17" s="1">
+        <v>16</v>
       </c>
       <c r="AA17" s="29"/>
       <c r="AB17" s="30"/>
@@ -6830,8 +6830,8 @@
       <c r="AI17" s="30"/>
       <c r="AJ17" s="31"/>
       <c r="AK17" s="45"/>
-      <c r="AL17" s="45">
-        <v>6</v>
+      <c r="AL17" s="1">
+        <v>16</v>
       </c>
       <c r="AM17" s="29"/>
       <c r="AN17" s="30"/>
@@ -6871,8 +6871,8 @@
     </row>
     <row r="18" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="45"/>
-      <c r="B18" s="45">
-        <v>5</v>
+      <c r="B18" s="1">
+        <v>17</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="30"/>
@@ -6885,8 +6885,8 @@
       <c r="K18" s="30"/>
       <c r="L18" s="31"/>
       <c r="M18" s="45"/>
-      <c r="N18" s="45">
-        <v>5</v>
+      <c r="N18" s="1">
+        <v>17</v>
       </c>
       <c r="O18" s="29"/>
       <c r="P18" s="30"/>
@@ -6899,8 +6899,8 @@
       <c r="W18" s="30"/>
       <c r="X18" s="31"/>
       <c r="Y18" s="45"/>
-      <c r="Z18" s="45">
-        <v>5</v>
+      <c r="Z18" s="1">
+        <v>17</v>
       </c>
       <c r="AA18" s="29"/>
       <c r="AB18" s="30"/>
@@ -6913,8 +6913,8 @@
       <c r="AI18" s="30"/>
       <c r="AJ18" s="31"/>
       <c r="AK18" s="45"/>
-      <c r="AL18" s="45">
-        <v>5</v>
+      <c r="AL18" s="1">
+        <v>17</v>
       </c>
       <c r="AM18" s="29"/>
       <c r="AN18" s="30"/>
@@ -6954,8 +6954,8 @@
     </row>
     <row r="19" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="45"/>
-      <c r="B19" s="45">
-        <v>4</v>
+      <c r="B19" s="1">
+        <v>18</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="30"/>
@@ -6968,8 +6968,8 @@
       <c r="K19" s="30"/>
       <c r="L19" s="31"/>
       <c r="M19" s="45"/>
-      <c r="N19" s="45">
-        <v>4</v>
+      <c r="N19" s="1">
+        <v>18</v>
       </c>
       <c r="O19" s="29"/>
       <c r="P19" s="30"/>
@@ -6982,8 +6982,8 @@
       <c r="W19" s="30"/>
       <c r="X19" s="31"/>
       <c r="Y19" s="45"/>
-      <c r="Z19" s="45">
-        <v>4</v>
+      <c r="Z19" s="1">
+        <v>18</v>
       </c>
       <c r="AA19" s="29"/>
       <c r="AB19" s="30"/>
@@ -6996,8 +6996,8 @@
       <c r="AI19" s="30"/>
       <c r="AJ19" s="31"/>
       <c r="AK19" s="45"/>
-      <c r="AL19" s="45">
-        <v>4</v>
+      <c r="AL19" s="1">
+        <v>18</v>
       </c>
       <c r="AM19" s="29"/>
       <c r="AN19" s="30"/>
@@ -7037,8 +7037,8 @@
     </row>
     <row r="20" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="45"/>
-      <c r="B20" s="45">
-        <v>3</v>
+      <c r="B20" s="1">
+        <v>19</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="30"/>
@@ -7051,8 +7051,8 @@
       <c r="K20" s="30"/>
       <c r="L20" s="31"/>
       <c r="M20" s="45"/>
-      <c r="N20" s="45">
-        <v>3</v>
+      <c r="N20" s="1">
+        <v>19</v>
       </c>
       <c r="O20" s="29"/>
       <c r="P20" s="30"/>
@@ -7065,8 +7065,8 @@
       <c r="W20" s="30"/>
       <c r="X20" s="31"/>
       <c r="Y20" s="45"/>
-      <c r="Z20" s="45">
-        <v>3</v>
+      <c r="Z20" s="1">
+        <v>19</v>
       </c>
       <c r="AA20" s="29"/>
       <c r="AB20" s="30"/>
@@ -7079,8 +7079,8 @@
       <c r="AI20" s="30"/>
       <c r="AJ20" s="31"/>
       <c r="AK20" s="45"/>
-      <c r="AL20" s="45">
-        <v>3</v>
+      <c r="AL20" s="1">
+        <v>19</v>
       </c>
       <c r="AM20" s="29"/>
       <c r="AN20" s="30"/>
@@ -7120,8 +7120,8 @@
     </row>
     <row r="21" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="45"/>
-      <c r="B21" s="45">
-        <v>2</v>
+      <c r="B21" s="1">
+        <v>20</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="30"/>
@@ -7134,8 +7134,8 @@
       <c r="K21" s="30"/>
       <c r="L21" s="31"/>
       <c r="M21" s="45"/>
-      <c r="N21" s="45">
-        <v>2</v>
+      <c r="N21" s="1">
+        <v>20</v>
       </c>
       <c r="O21" s="29"/>
       <c r="P21" s="30"/>
@@ -7148,8 +7148,8 @@
       <c r="W21" s="30"/>
       <c r="X21" s="31"/>
       <c r="Y21" s="45"/>
-      <c r="Z21" s="45">
-        <v>2</v>
+      <c r="Z21" s="1">
+        <v>20</v>
       </c>
       <c r="AA21" s="29"/>
       <c r="AB21" s="30"/>
@@ -7162,8 +7162,8 @@
       <c r="AI21" s="30"/>
       <c r="AJ21" s="31"/>
       <c r="AK21" s="45"/>
-      <c r="AL21" s="45">
-        <v>2</v>
+      <c r="AL21" s="1">
+        <v>20</v>
       </c>
       <c r="AM21" s="29"/>
       <c r="AN21" s="30"/>
@@ -7203,8 +7203,8 @@
     </row>
     <row r="22" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="45"/>
-      <c r="B22" s="45">
-        <v>1</v>
+      <c r="B22" s="1">
+        <v>21</v>
       </c>
       <c r="C22" s="29"/>
       <c r="D22" s="30"/>
@@ -7217,8 +7217,8 @@
       <c r="K22" s="30"/>
       <c r="L22" s="31"/>
       <c r="M22" s="45"/>
-      <c r="N22" s="45">
-        <v>1</v>
+      <c r="N22" s="1">
+        <v>21</v>
       </c>
       <c r="O22" s="29"/>
       <c r="P22" s="30"/>
@@ -7231,8 +7231,8 @@
       <c r="W22" s="30"/>
       <c r="X22" s="31"/>
       <c r="Y22" s="45"/>
-      <c r="Z22" s="45">
-        <v>1</v>
+      <c r="Z22" s="1">
+        <v>21</v>
       </c>
       <c r="AA22" s="29"/>
       <c r="AB22" s="30"/>
@@ -7245,8 +7245,8 @@
       <c r="AI22" s="30"/>
       <c r="AJ22" s="31"/>
       <c r="AK22" s="45"/>
-      <c r="AL22" s="45">
-        <v>1</v>
+      <c r="AL22" s="1">
+        <v>21</v>
       </c>
       <c r="AM22" s="29"/>
       <c r="AN22" s="30"/>
@@ -7286,8 +7286,8 @@
     </row>
     <row r="23" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="45"/>
-      <c r="B23" s="45">
-        <v>0</v>
+      <c r="B23" s="1">
+        <v>22</v>
       </c>
       <c r="C23" s="32"/>
       <c r="D23" s="33"/>
@@ -7300,8 +7300,8 @@
       <c r="K23" s="33"/>
       <c r="L23" s="34"/>
       <c r="M23" s="45"/>
-      <c r="N23" s="45">
-        <v>0</v>
+      <c r="N23" s="1">
+        <v>22</v>
       </c>
       <c r="O23" s="32"/>
       <c r="P23" s="33"/>
@@ -7314,8 +7314,8 @@
       <c r="W23" s="33"/>
       <c r="X23" s="34"/>
       <c r="Y23" s="45"/>
-      <c r="Z23" s="45">
-        <v>0</v>
+      <c r="Z23" s="1">
+        <v>22</v>
       </c>
       <c r="AA23" s="32"/>
       <c r="AB23" s="33"/>
@@ -7328,8 +7328,8 @@
       <c r="AI23" s="33"/>
       <c r="AJ23" s="34"/>
       <c r="AK23" s="45"/>
-      <c r="AL23" s="45">
-        <v>0</v>
+      <c r="AL23" s="1">
+        <v>22</v>
       </c>
       <c r="AM23" s="32"/>
       <c r="AN23" s="33"/>
@@ -7371,130 +7371,130 @@
       <c r="A24" s="45"/>
       <c r="B24" s="45"/>
       <c r="C24" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" s="45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" s="45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G24" s="45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H24" s="45">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I24" s="45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J24" s="45">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K24" s="45">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L24" s="45">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M24" s="45"/>
       <c r="N24" s="45"/>
       <c r="O24" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24" s="45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q24" s="45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R24" s="45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S24" s="45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T24" s="45">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U24" s="45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V24" s="45">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="W24" s="45">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X24" s="45">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Y24" s="45"/>
       <c r="Z24" s="45"/>
       <c r="AA24" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB24" s="45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC24" s="45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD24" s="45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE24" s="45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AF24" s="45">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AG24" s="45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AH24" s="45">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AI24" s="45">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AJ24" s="45">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AK24" s="45"/>
       <c r="AL24" s="45"/>
       <c r="AM24" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN24" s="45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AO24" s="45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AP24" s="45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AQ24" s="45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AR24" s="45">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AS24" s="45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AT24" s="45">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AU24" s="45">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AV24" s="45">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AW24" s="45"/>
       <c r="AX24" s="1"/>
@@ -7599,8 +7599,8 @@
     </row>
     <row r="26" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="45"/>
-      <c r="B26" s="45">
-        <v>21</v>
+      <c r="B26" s="1">
+        <v>1</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="20"/>
@@ -7617,8 +7617,8 @@
       <c r="K26" s="20"/>
       <c r="L26" s="21"/>
       <c r="M26" s="45"/>
-      <c r="N26" s="45">
-        <v>21</v>
+      <c r="N26" s="1">
+        <v>1</v>
       </c>
       <c r="O26" s="19"/>
       <c r="P26" s="20"/>
@@ -7633,8 +7633,8 @@
       <c r="W26" s="20"/>
       <c r="X26" s="21"/>
       <c r="Y26" s="45"/>
-      <c r="Z26" s="45">
-        <v>21</v>
+      <c r="Z26" s="1">
+        <v>1</v>
       </c>
       <c r="AA26" s="19"/>
       <c r="AB26" s="20"/>
@@ -7690,8 +7690,8 @@
     </row>
     <row r="27" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="45"/>
-      <c r="B27" s="45">
-        <v>20</v>
+      <c r="B27" s="1">
+        <v>2</v>
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="23"/>
@@ -7708,8 +7708,8 @@
       <c r="K27" s="23"/>
       <c r="L27" s="25"/>
       <c r="M27" s="45"/>
-      <c r="N27" s="45">
-        <v>20</v>
+      <c r="N27" s="1">
+        <v>2</v>
       </c>
       <c r="O27" s="22"/>
       <c r="P27" s="23"/>
@@ -7728,8 +7728,8 @@
       <c r="W27" s="23"/>
       <c r="X27" s="25"/>
       <c r="Y27" s="45"/>
-      <c r="Z27" s="45">
-        <v>20</v>
+      <c r="Z27" s="1">
+        <v>2</v>
       </c>
       <c r="AA27" s="22"/>
       <c r="AB27" s="23"/>
@@ -7785,8 +7785,8 @@
     </row>
     <row r="28" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="45"/>
-      <c r="B28" s="45">
-        <v>19</v>
+      <c r="B28" s="1">
+        <v>3</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="27"/>
@@ -7799,8 +7799,8 @@
       <c r="K28" s="27"/>
       <c r="L28" s="28"/>
       <c r="M28" s="45"/>
-      <c r="N28" s="45">
-        <v>19</v>
+      <c r="N28" s="1">
+        <v>3</v>
       </c>
       <c r="O28" s="26"/>
       <c r="P28" s="27"/>
@@ -7813,8 +7813,8 @@
       <c r="W28" s="27"/>
       <c r="X28" s="28"/>
       <c r="Y28" s="45"/>
-      <c r="Z28" s="45">
-        <v>19</v>
+      <c r="Z28" s="1">
+        <v>3</v>
       </c>
       <c r="AA28" s="26"/>
       <c r="AB28" s="27"/>
@@ -7866,8 +7866,8 @@
     </row>
     <row r="29" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="45"/>
-      <c r="B29" s="45">
-        <v>18</v>
+      <c r="B29" s="1">
+        <v>4</v>
       </c>
       <c r="C29" s="29"/>
       <c r="D29" s="30"/>
@@ -7880,8 +7880,8 @@
       <c r="K29" s="30"/>
       <c r="L29" s="31"/>
       <c r="M29" s="45"/>
-      <c r="N29" s="45">
-        <v>18</v>
+      <c r="N29" s="1">
+        <v>4</v>
       </c>
       <c r="O29" s="29"/>
       <c r="P29" s="30"/>
@@ -7894,8 +7894,8 @@
       <c r="W29" s="30"/>
       <c r="X29" s="31"/>
       <c r="Y29" s="45"/>
-      <c r="Z29" s="45">
-        <v>18</v>
+      <c r="Z29" s="1">
+        <v>4</v>
       </c>
       <c r="AA29" s="29"/>
       <c r="AB29" s="30"/>
@@ -7947,8 +7947,8 @@
     </row>
     <row r="30" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="45"/>
-      <c r="B30" s="45">
-        <v>17</v>
+      <c r="B30" s="1">
+        <v>5</v>
       </c>
       <c r="C30" s="29"/>
       <c r="D30" s="30"/>
@@ -7961,8 +7961,8 @@
       <c r="K30" s="30"/>
       <c r="L30" s="31"/>
       <c r="M30" s="45"/>
-      <c r="N30" s="45">
-        <v>17</v>
+      <c r="N30" s="1">
+        <v>5</v>
       </c>
       <c r="O30" s="29"/>
       <c r="P30" s="30"/>
@@ -7975,8 +7975,8 @@
       <c r="W30" s="30"/>
       <c r="X30" s="31"/>
       <c r="Y30" s="45"/>
-      <c r="Z30" s="45">
-        <v>17</v>
+      <c r="Z30" s="1">
+        <v>5</v>
       </c>
       <c r="AA30" s="29"/>
       <c r="AB30" s="30"/>
@@ -8028,8 +8028,8 @@
     </row>
     <row r="31" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="45"/>
-      <c r="B31" s="45">
-        <v>16</v>
+      <c r="B31" s="1">
+        <v>6</v>
       </c>
       <c r="C31" s="29"/>
       <c r="D31" s="30"/>
@@ -8042,8 +8042,8 @@
       <c r="K31" s="30"/>
       <c r="L31" s="31"/>
       <c r="M31" s="45"/>
-      <c r="N31" s="45">
-        <v>16</v>
+      <c r="N31" s="1">
+        <v>6</v>
       </c>
       <c r="O31" s="29"/>
       <c r="P31" s="30"/>
@@ -8056,8 +8056,8 @@
       <c r="W31" s="30"/>
       <c r="X31" s="31"/>
       <c r="Y31" s="45"/>
-      <c r="Z31" s="45">
-        <v>16</v>
+      <c r="Z31" s="1">
+        <v>6</v>
       </c>
       <c r="AA31" s="29"/>
       <c r="AB31" s="30"/>
@@ -8109,8 +8109,8 @@
     </row>
     <row r="32" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="45"/>
-      <c r="B32" s="45">
-        <v>15</v>
+      <c r="B32" s="1">
+        <v>7</v>
       </c>
       <c r="C32" s="29"/>
       <c r="D32" s="30"/>
@@ -8123,8 +8123,8 @@
       <c r="K32" s="30"/>
       <c r="L32" s="31"/>
       <c r="M32" s="45"/>
-      <c r="N32" s="45">
-        <v>15</v>
+      <c r="N32" s="1">
+        <v>7</v>
       </c>
       <c r="O32" s="29"/>
       <c r="P32" s="30"/>
@@ -8137,8 +8137,8 @@
       <c r="W32" s="30"/>
       <c r="X32" s="31"/>
       <c r="Y32" s="45"/>
-      <c r="Z32" s="45">
-        <v>15</v>
+      <c r="Z32" s="1">
+        <v>7</v>
       </c>
       <c r="AA32" s="29"/>
       <c r="AB32" s="30"/>
@@ -8190,8 +8190,8 @@
     </row>
     <row r="33" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="45"/>
-      <c r="B33" s="45">
-        <v>14</v>
+      <c r="B33" s="1">
+        <v>8</v>
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="30"/>
@@ -8204,8 +8204,8 @@
       <c r="K33" s="30"/>
       <c r="L33" s="31"/>
       <c r="M33" s="45"/>
-      <c r="N33" s="45">
-        <v>14</v>
+      <c r="N33" s="1">
+        <v>8</v>
       </c>
       <c r="O33" s="29"/>
       <c r="P33" s="30"/>
@@ -8218,8 +8218,8 @@
       <c r="W33" s="30"/>
       <c r="X33" s="31"/>
       <c r="Y33" s="45"/>
-      <c r="Z33" s="45">
-        <v>14</v>
+      <c r="Z33" s="1">
+        <v>8</v>
       </c>
       <c r="AA33" s="29"/>
       <c r="AB33" s="30"/>
@@ -8271,8 +8271,8 @@
     </row>
     <row r="34" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="45"/>
-      <c r="B34" s="45">
-        <v>13</v>
+      <c r="B34" s="1">
+        <v>9</v>
       </c>
       <c r="C34" s="29"/>
       <c r="D34" s="30"/>
@@ -8285,8 +8285,8 @@
       <c r="K34" s="30"/>
       <c r="L34" s="31"/>
       <c r="M34" s="45"/>
-      <c r="N34" s="45">
-        <v>13</v>
+      <c r="N34" s="1">
+        <v>9</v>
       </c>
       <c r="O34" s="29"/>
       <c r="P34" s="30"/>
@@ -8299,8 +8299,8 @@
       <c r="W34" s="30"/>
       <c r="X34" s="31"/>
       <c r="Y34" s="45"/>
-      <c r="Z34" s="45">
-        <v>13</v>
+      <c r="Z34" s="1">
+        <v>9</v>
       </c>
       <c r="AA34" s="29"/>
       <c r="AB34" s="30"/>
@@ -8352,8 +8352,8 @@
     </row>
     <row r="35" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="45"/>
-      <c r="B35" s="45">
-        <v>12</v>
+      <c r="B35" s="1">
+        <v>10</v>
       </c>
       <c r="C35" s="29"/>
       <c r="D35" s="30"/>
@@ -8366,8 +8366,8 @@
       <c r="K35" s="30"/>
       <c r="L35" s="31"/>
       <c r="M35" s="45"/>
-      <c r="N35" s="45">
-        <v>12</v>
+      <c r="N35" s="1">
+        <v>10</v>
       </c>
       <c r="O35" s="29"/>
       <c r="P35" s="30"/>
@@ -8380,8 +8380,8 @@
       <c r="W35" s="30"/>
       <c r="X35" s="31"/>
       <c r="Y35" s="45"/>
-      <c r="Z35" s="45">
-        <v>12</v>
+      <c r="Z35" s="1">
+        <v>10</v>
       </c>
       <c r="AA35" s="29"/>
       <c r="AB35" s="30"/>
@@ -8433,7 +8433,7 @@
     </row>
     <row r="36" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="45"/>
-      <c r="B36" s="45">
+      <c r="B36" s="1">
         <v>11</v>
       </c>
       <c r="C36" s="29"/>
@@ -8447,7 +8447,7 @@
       <c r="K36" s="30"/>
       <c r="L36" s="31"/>
       <c r="M36" s="45"/>
-      <c r="N36" s="45">
+      <c r="N36" s="1">
         <v>11</v>
       </c>
       <c r="O36" s="29"/>
@@ -8461,7 +8461,7 @@
       <c r="W36" s="30"/>
       <c r="X36" s="31"/>
       <c r="Y36" s="45"/>
-      <c r="Z36" s="45">
+      <c r="Z36" s="1">
         <v>11</v>
       </c>
       <c r="AA36" s="29"/>
@@ -8514,8 +8514,8 @@
     </row>
     <row r="37" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="45"/>
-      <c r="B37" s="45">
-        <v>10</v>
+      <c r="B37" s="1">
+        <v>12</v>
       </c>
       <c r="C37" s="29"/>
       <c r="D37" s="30"/>
@@ -8528,8 +8528,8 @@
       <c r="K37" s="30"/>
       <c r="L37" s="31"/>
       <c r="M37" s="45"/>
-      <c r="N37" s="45">
-        <v>10</v>
+      <c r="N37" s="1">
+        <v>12</v>
       </c>
       <c r="O37" s="29"/>
       <c r="P37" s="30"/>
@@ -8542,8 +8542,8 @@
       <c r="W37" s="30"/>
       <c r="X37" s="31"/>
       <c r="Y37" s="45"/>
-      <c r="Z37" s="45">
-        <v>10</v>
+      <c r="Z37" s="1">
+        <v>12</v>
       </c>
       <c r="AA37" s="29"/>
       <c r="AB37" s="30"/>
@@ -8595,8 +8595,8 @@
     </row>
     <row r="38" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="45"/>
-      <c r="B38" s="45">
-        <v>9</v>
+      <c r="B38" s="1">
+        <v>13</v>
       </c>
       <c r="C38" s="29"/>
       <c r="D38" s="30"/>
@@ -8609,8 +8609,8 @@
       <c r="K38" s="30"/>
       <c r="L38" s="31"/>
       <c r="M38" s="45"/>
-      <c r="N38" s="45">
-        <v>9</v>
+      <c r="N38" s="1">
+        <v>13</v>
       </c>
       <c r="O38" s="29"/>
       <c r="P38" s="30"/>
@@ -8623,8 +8623,8 @@
       <c r="W38" s="30"/>
       <c r="X38" s="31"/>
       <c r="Y38" s="45"/>
-      <c r="Z38" s="45">
-        <v>9</v>
+      <c r="Z38" s="1">
+        <v>13</v>
       </c>
       <c r="AA38" s="29"/>
       <c r="AB38" s="30"/>
@@ -8676,8 +8676,8 @@
     </row>
     <row r="39" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="45"/>
-      <c r="B39" s="45">
-        <v>8</v>
+      <c r="B39" s="1">
+        <v>14</v>
       </c>
       <c r="C39" s="29"/>
       <c r="D39" s="30"/>
@@ -8690,8 +8690,8 @@
       <c r="K39" s="30"/>
       <c r="L39" s="31"/>
       <c r="M39" s="45"/>
-      <c r="N39" s="45">
-        <v>8</v>
+      <c r="N39" s="1">
+        <v>14</v>
       </c>
       <c r="O39" s="29"/>
       <c r="P39" s="30"/>
@@ -8704,8 +8704,8 @@
       <c r="W39" s="30"/>
       <c r="X39" s="31"/>
       <c r="Y39" s="45"/>
-      <c r="Z39" s="45">
-        <v>8</v>
+      <c r="Z39" s="1">
+        <v>14</v>
       </c>
       <c r="AA39" s="29"/>
       <c r="AB39" s="30"/>
@@ -8757,8 +8757,8 @@
     </row>
     <row r="40" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="45"/>
-      <c r="B40" s="45">
-        <v>7</v>
+      <c r="B40" s="1">
+        <v>15</v>
       </c>
       <c r="C40" s="29"/>
       <c r="D40" s="30"/>
@@ -8771,8 +8771,8 @@
       <c r="K40" s="30"/>
       <c r="L40" s="31"/>
       <c r="M40" s="45"/>
-      <c r="N40" s="45">
-        <v>7</v>
+      <c r="N40" s="1">
+        <v>15</v>
       </c>
       <c r="O40" s="29"/>
       <c r="P40" s="30"/>
@@ -8785,8 +8785,8 @@
       <c r="W40" s="30"/>
       <c r="X40" s="31"/>
       <c r="Y40" s="45"/>
-      <c r="Z40" s="45">
-        <v>7</v>
+      <c r="Z40" s="1">
+        <v>15</v>
       </c>
       <c r="AA40" s="29"/>
       <c r="AB40" s="30"/>
@@ -8838,8 +8838,8 @@
     </row>
     <row r="41" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="45"/>
-      <c r="B41" s="45">
-        <v>6</v>
+      <c r="B41" s="1">
+        <v>16</v>
       </c>
       <c r="C41" s="29"/>
       <c r="D41" s="30"/>
@@ -8852,8 +8852,8 @@
       <c r="K41" s="30"/>
       <c r="L41" s="31"/>
       <c r="M41" s="45"/>
-      <c r="N41" s="45">
-        <v>6</v>
+      <c r="N41" s="1">
+        <v>16</v>
       </c>
       <c r="O41" s="29"/>
       <c r="P41" s="30"/>
@@ -8866,8 +8866,8 @@
       <c r="W41" s="30"/>
       <c r="X41" s="31"/>
       <c r="Y41" s="45"/>
-      <c r="Z41" s="45">
-        <v>6</v>
+      <c r="Z41" s="1">
+        <v>16</v>
       </c>
       <c r="AA41" s="29"/>
       <c r="AB41" s="30"/>
@@ -8919,8 +8919,8 @@
     </row>
     <row r="42" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="45"/>
-      <c r="B42" s="45">
-        <v>5</v>
+      <c r="B42" s="1">
+        <v>17</v>
       </c>
       <c r="C42" s="29"/>
       <c r="D42" s="30"/>
@@ -8933,8 +8933,8 @@
       <c r="K42" s="30"/>
       <c r="L42" s="31"/>
       <c r="M42" s="45"/>
-      <c r="N42" s="45">
-        <v>5</v>
+      <c r="N42" s="1">
+        <v>17</v>
       </c>
       <c r="O42" s="29"/>
       <c r="P42" s="30"/>
@@ -8947,8 +8947,8 @@
       <c r="W42" s="30"/>
       <c r="X42" s="31"/>
       <c r="Y42" s="45"/>
-      <c r="Z42" s="45">
-        <v>5</v>
+      <c r="Z42" s="1">
+        <v>17</v>
       </c>
       <c r="AA42" s="29"/>
       <c r="AB42" s="30"/>
@@ -9000,8 +9000,8 @@
     </row>
     <row r="43" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="45"/>
-      <c r="B43" s="45">
-        <v>4</v>
+      <c r="B43" s="1">
+        <v>18</v>
       </c>
       <c r="C43" s="29"/>
       <c r="D43" s="30"/>
@@ -9014,8 +9014,8 @@
       <c r="K43" s="30"/>
       <c r="L43" s="31"/>
       <c r="M43" s="45"/>
-      <c r="N43" s="45">
-        <v>4</v>
+      <c r="N43" s="1">
+        <v>18</v>
       </c>
       <c r="O43" s="29"/>
       <c r="P43" s="30"/>
@@ -9028,8 +9028,8 @@
       <c r="W43" s="30"/>
       <c r="X43" s="31"/>
       <c r="Y43" s="45"/>
-      <c r="Z43" s="45">
-        <v>4</v>
+      <c r="Z43" s="1">
+        <v>18</v>
       </c>
       <c r="AA43" s="29"/>
       <c r="AB43" s="30"/>
@@ -9081,8 +9081,8 @@
     </row>
     <row r="44" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="45"/>
-      <c r="B44" s="45">
-        <v>3</v>
+      <c r="B44" s="1">
+        <v>19</v>
       </c>
       <c r="C44" s="29"/>
       <c r="D44" s="30"/>
@@ -9095,8 +9095,8 @@
       <c r="K44" s="30"/>
       <c r="L44" s="31"/>
       <c r="M44" s="45"/>
-      <c r="N44" s="45">
-        <v>3</v>
+      <c r="N44" s="1">
+        <v>19</v>
       </c>
       <c r="O44" s="29"/>
       <c r="P44" s="30"/>
@@ -9109,8 +9109,8 @@
       <c r="W44" s="30"/>
       <c r="X44" s="31"/>
       <c r="Y44" s="45"/>
-      <c r="Z44" s="45">
-        <v>3</v>
+      <c r="Z44" s="1">
+        <v>19</v>
       </c>
       <c r="AA44" s="29"/>
       <c r="AB44" s="30"/>
@@ -9162,8 +9162,8 @@
     </row>
     <row r="45" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="45"/>
-      <c r="B45" s="45">
-        <v>2</v>
+      <c r="B45" s="1">
+        <v>20</v>
       </c>
       <c r="C45" s="29"/>
       <c r="D45" s="30"/>
@@ -9176,8 +9176,8 @@
       <c r="K45" s="30"/>
       <c r="L45" s="31"/>
       <c r="M45" s="45"/>
-      <c r="N45" s="45">
-        <v>2</v>
+      <c r="N45" s="1">
+        <v>20</v>
       </c>
       <c r="O45" s="29"/>
       <c r="P45" s="30"/>
@@ -9190,8 +9190,8 @@
       <c r="W45" s="30"/>
       <c r="X45" s="31"/>
       <c r="Y45" s="45"/>
-      <c r="Z45" s="45">
-        <v>2</v>
+      <c r="Z45" s="1">
+        <v>20</v>
       </c>
       <c r="AA45" s="29"/>
       <c r="AB45" s="30"/>
@@ -9243,8 +9243,8 @@
     </row>
     <row r="46" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="45"/>
-      <c r="B46" s="45">
-        <v>1</v>
+      <c r="B46" s="1">
+        <v>21</v>
       </c>
       <c r="C46" s="29"/>
       <c r="D46" s="30"/>
@@ -9257,8 +9257,8 @@
       <c r="K46" s="30"/>
       <c r="L46" s="31"/>
       <c r="M46" s="45"/>
-      <c r="N46" s="45">
-        <v>1</v>
+      <c r="N46" s="1">
+        <v>21</v>
       </c>
       <c r="O46" s="29"/>
       <c r="P46" s="30"/>
@@ -9271,8 +9271,8 @@
       <c r="W46" s="30"/>
       <c r="X46" s="31"/>
       <c r="Y46" s="45"/>
-      <c r="Z46" s="45">
-        <v>1</v>
+      <c r="Z46" s="1">
+        <v>21</v>
       </c>
       <c r="AA46" s="29"/>
       <c r="AB46" s="30"/>
@@ -9324,8 +9324,8 @@
     </row>
     <row r="47" spans="1:73" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="45"/>
-      <c r="B47" s="45">
-        <v>0</v>
+      <c r="B47" s="1">
+        <v>22</v>
       </c>
       <c r="C47" s="32"/>
       <c r="D47" s="33"/>
@@ -9338,8 +9338,8 @@
       <c r="K47" s="33"/>
       <c r="L47" s="34"/>
       <c r="M47" s="45"/>
-      <c r="N47" s="45">
-        <v>0</v>
+      <c r="N47" s="1">
+        <v>22</v>
       </c>
       <c r="O47" s="32"/>
       <c r="P47" s="33"/>
@@ -9352,8 +9352,8 @@
       <c r="W47" s="33"/>
       <c r="X47" s="34"/>
       <c r="Y47" s="45"/>
-      <c r="Z47" s="45">
-        <v>0</v>
+      <c r="Z47" s="1">
+        <v>22</v>
       </c>
       <c r="AA47" s="32"/>
       <c r="AB47" s="33"/>
@@ -9407,98 +9407,98 @@
       <c r="A48" s="45"/>
       <c r="B48" s="45"/>
       <c r="C48" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" s="45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E48" s="45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F48" s="45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G48" s="45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H48" s="45">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I48" s="45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J48" s="45">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K48" s="45">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L48" s="45">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M48" s="45"/>
       <c r="N48" s="45"/>
       <c r="O48" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P48" s="45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q48" s="45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R48" s="45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S48" s="45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T48" s="45">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U48" s="45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V48" s="45">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="W48" s="45">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X48" s="45">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Y48" s="45"/>
       <c r="Z48" s="45"/>
       <c r="AA48" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB48" s="45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC48" s="45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD48" s="45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE48" s="45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AF48" s="45">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AG48" s="45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AH48" s="45">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AI48" s="45">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AJ48" s="45">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AK48" s="45"/>
       <c r="AL48" s="45"/>
@@ -11947,8 +11947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BY82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z45" sqref="Z45"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed mino numbers in excel
</commit_message>
<xml_diff>
--- a/tetris.xlsx
+++ b/tetris.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14840" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="30840" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="board" sheetId="1" r:id="rId1"/>
@@ -501,12 +501,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -566,6 +560,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB80"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5425,8 +5425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU80"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48:L48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AF27" sqref="AF27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5532,7 +5532,7 @@
       <c r="P2" s="20"/>
       <c r="Q2" s="20"/>
       <c r="R2" s="47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2" s="46"/>
       <c r="T2" s="46"/>
@@ -5550,7 +5550,7 @@
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
       <c r="AF2" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG2" s="20"/>
       <c r="AH2" s="20"/>
@@ -5565,10 +5565,10 @@
       <c r="AO2" s="20"/>
       <c r="AP2" s="20"/>
       <c r="AQ2" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR2" s="37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AS2" s="20"/>
       <c r="AT2" s="20"/>
@@ -5609,16 +5609,16 @@
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
       <c r="F3" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="23"/>
@@ -5631,13 +5631,13 @@
       <c r="P3" s="23"/>
       <c r="Q3" s="23"/>
       <c r="R3" s="48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S3" s="48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T3" s="48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U3" s="23"/>
       <c r="V3" s="23"/>
@@ -5651,13 +5651,13 @@
       <c r="AB3" s="23"/>
       <c r="AC3" s="23"/>
       <c r="AD3" s="36">
+        <v>4</v>
+      </c>
+      <c r="AE3" s="36">
         <v>3</v>
       </c>
-      <c r="AE3" s="36">
+      <c r="AF3" s="36">
         <v>2</v>
-      </c>
-      <c r="AF3" s="36">
-        <v>1</v>
       </c>
       <c r="AG3" s="23"/>
       <c r="AH3" s="23"/>
@@ -5672,10 +5672,10 @@
       <c r="AO3" s="23"/>
       <c r="AP3" s="23"/>
       <c r="AQ3" s="38">
+        <v>4</v>
+      </c>
+      <c r="AR3" s="38">
         <v>3</v>
-      </c>
-      <c r="AR3" s="38">
-        <v>2</v>
       </c>
       <c r="AS3" s="23"/>
       <c r="AT3" s="23"/>
@@ -7607,10 +7607,10 @@
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="39">
+        <v>2</v>
+      </c>
+      <c r="H26" s="39">
         <v>1</v>
-      </c>
-      <c r="H26" s="39">
-        <v>0</v>
       </c>
       <c r="I26" s="20"/>
       <c r="J26" s="20"/>
@@ -7625,7 +7625,7 @@
       <c r="Q26" s="20"/>
       <c r="R26" s="20"/>
       <c r="S26" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T26" s="20"/>
       <c r="U26" s="20"/>
@@ -7640,10 +7640,10 @@
       <c r="AB26" s="20"/>
       <c r="AC26" s="20"/>
       <c r="AD26" s="43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE26" s="43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF26" s="20"/>
       <c r="AG26" s="20"/>
@@ -7697,10 +7697,10 @@
       <c r="D27" s="23"/>
       <c r="E27" s="23"/>
       <c r="F27" s="40">
+        <v>4</v>
+      </c>
+      <c r="G27" s="40">
         <v>3</v>
-      </c>
-      <c r="G27" s="40">
-        <v>2</v>
       </c>
       <c r="H27" s="23"/>
       <c r="I27" s="23"/>
@@ -7715,13 +7715,13 @@
       <c r="P27" s="23"/>
       <c r="Q27" s="23"/>
       <c r="R27" s="42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S27" s="42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T27" s="42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U27" s="23"/>
       <c r="V27" s="23"/>
@@ -7736,10 +7736,10 @@
       <c r="AC27" s="23"/>
       <c r="AD27" s="23"/>
       <c r="AE27" s="44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF27" s="44">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG27" s="23"/>
       <c r="AH27" s="23"/>
@@ -11947,8 +11947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BY82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12037,39 +12037,39 @@
     </row>
     <row r="2" spans="1:77" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="55">
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="75">
         <v>0</v>
       </c>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
       <c r="J2" s="54"/>
-      <c r="K2" s="55">
+      <c r="K2" s="75">
         <v>1</v>
       </c>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
       <c r="O2" s="54"/>
-      <c r="P2" s="55">
+      <c r="P2" s="75">
         <v>2</v>
       </c>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
       <c r="T2" s="54"/>
-      <c r="U2" s="55">
+      <c r="U2" s="75">
         <v>3</v>
       </c>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
       <c r="Y2" s="45"/>
       <c r="Z2" s="45"/>
       <c r="AA2" s="45"/>
@@ -12217,7 +12217,7 @@
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
       <c r="M4" s="52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="28"/>
       <c r="O4" s="45"/>
@@ -12228,7 +12228,7 @@
       <c r="T4" s="45"/>
       <c r="U4" s="26"/>
       <c r="V4" s="52">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W4" s="27"/>
       <c r="X4" s="28"/>
@@ -12293,22 +12293,22 @@
       <c r="D5" s="1"/>
       <c r="E5" s="45"/>
       <c r="F5" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" s="50">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I5" s="51">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J5" s="45"/>
       <c r="K5" s="29"/>
       <c r="L5" s="30"/>
       <c r="M5" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N5" s="31"/>
       <c r="O5" s="45"/>
@@ -12319,7 +12319,7 @@
       <c r="T5" s="45"/>
       <c r="U5" s="29"/>
       <c r="V5" s="50">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W5" s="30"/>
       <c r="X5" s="31"/>
@@ -12391,26 +12391,26 @@
       <c r="K6" s="29"/>
       <c r="L6" s="30"/>
       <c r="M6" s="50">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N6" s="31"/>
       <c r="O6" s="45"/>
       <c r="P6" s="49">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="50">
         <v>3</v>
       </c>
-      <c r="Q6" s="50">
+      <c r="R6" s="50">
         <v>2</v>
       </c>
-      <c r="R6" s="50">
+      <c r="S6" s="51">
         <v>1</v>
-      </c>
-      <c r="S6" s="51">
-        <v>0</v>
       </c>
       <c r="T6" s="45"/>
       <c r="U6" s="29"/>
       <c r="V6" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W6" s="30"/>
       <c r="X6" s="31"/>
@@ -12482,7 +12482,7 @@
       <c r="K7" s="32"/>
       <c r="L7" s="33"/>
       <c r="M7" s="53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N7" s="34"/>
       <c r="O7" s="45"/>
@@ -12493,7 +12493,7 @@
       <c r="T7" s="45"/>
       <c r="U7" s="32"/>
       <c r="V7" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" s="33"/>
       <c r="X7" s="34"/>
@@ -12636,19 +12636,19 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="45"/>
-      <c r="F9" s="57">
-        <v>0</v>
+      <c r="F9" s="55">
+        <v>1</v>
       </c>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
       <c r="I9" s="28"/>
       <c r="J9" s="45"/>
       <c r="K9" s="26"/>
-      <c r="L9" s="60">
+      <c r="L9" s="58">
+        <v>2</v>
+      </c>
+      <c r="M9" s="58">
         <v>1</v>
-      </c>
-      <c r="M9" s="60">
-        <v>0</v>
       </c>
       <c r="N9" s="28"/>
       <c r="O9" s="45"/>
@@ -12658,8 +12658,8 @@
       <c r="S9" s="28"/>
       <c r="T9" s="45"/>
       <c r="U9" s="26"/>
-      <c r="V9" s="60">
-        <v>3</v>
+      <c r="V9" s="58">
+        <v>4</v>
       </c>
       <c r="W9" s="27"/>
       <c r="X9" s="28"/>
@@ -12723,38 +12723,38 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="45"/>
-      <c r="F10" s="58">
-        <v>1</v>
-      </c>
-      <c r="G10" s="59">
+      <c r="F10" s="56">
         <v>2</v>
       </c>
-      <c r="H10" s="59">
+      <c r="G10" s="57">
         <v>3</v>
+      </c>
+      <c r="H10" s="57">
+        <v>4</v>
       </c>
       <c r="I10" s="31"/>
       <c r="J10" s="45"/>
       <c r="K10" s="29"/>
-      <c r="L10" s="59">
-        <v>2</v>
+      <c r="L10" s="57">
+        <v>3</v>
       </c>
       <c r="M10" s="30"/>
       <c r="N10" s="31"/>
       <c r="O10" s="45"/>
-      <c r="P10" s="58">
+      <c r="P10" s="56">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="57">
         <v>3</v>
       </c>
-      <c r="Q10" s="59">
+      <c r="R10" s="57">
         <v>2</v>
-      </c>
-      <c r="R10" s="59">
-        <v>1</v>
       </c>
       <c r="S10" s="31"/>
       <c r="T10" s="45"/>
       <c r="U10" s="29"/>
-      <c r="V10" s="59">
-        <v>2</v>
+      <c r="V10" s="57">
+        <v>3</v>
       </c>
       <c r="W10" s="30"/>
       <c r="X10" s="31"/>
@@ -12824,24 +12824,24 @@
       <c r="I11" s="31"/>
       <c r="J11" s="45"/>
       <c r="K11" s="29"/>
-      <c r="L11" s="59">
-        <v>3</v>
+      <c r="L11" s="57">
+        <v>4</v>
       </c>
       <c r="M11" s="30"/>
       <c r="N11" s="31"/>
       <c r="O11" s="45"/>
       <c r="P11" s="29"/>
       <c r="Q11" s="30"/>
-      <c r="R11" s="59">
-        <v>0</v>
+      <c r="R11" s="57">
+        <v>1</v>
       </c>
       <c r="S11" s="31"/>
       <c r="T11" s="45"/>
-      <c r="U11" s="58">
-        <v>0</v>
-      </c>
-      <c r="V11" s="59">
+      <c r="U11" s="56">
         <v>1</v>
+      </c>
+      <c r="V11" s="57">
+        <v>2</v>
       </c>
       <c r="W11" s="30"/>
       <c r="X11" s="31"/>
@@ -13065,14 +13065,14 @@
       <c r="E14" s="45"/>
       <c r="F14" s="26"/>
       <c r="G14" s="27"/>
-      <c r="H14" s="64">
-        <v>0</v>
+      <c r="H14" s="62">
+        <v>1</v>
       </c>
       <c r="I14" s="28"/>
       <c r="J14" s="45"/>
       <c r="K14" s="26"/>
-      <c r="L14" s="64">
-        <v>3</v>
+      <c r="L14" s="62">
+        <v>4</v>
       </c>
       <c r="M14" s="27"/>
       <c r="N14" s="28"/>
@@ -13082,11 +13082,11 @@
       <c r="R14" s="27"/>
       <c r="S14" s="28"/>
       <c r="T14" s="45"/>
-      <c r="U14" s="65">
-        <v>0</v>
-      </c>
-      <c r="V14" s="64">
+      <c r="U14" s="63">
         <v>1</v>
+      </c>
+      <c r="V14" s="62">
+        <v>2</v>
       </c>
       <c r="W14" s="27"/>
       <c r="X14" s="28"/>
@@ -13150,38 +13150,38 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="45"/>
-      <c r="F15" s="62">
+      <c r="F15" s="60">
+        <v>4</v>
+      </c>
+      <c r="G15" s="61">
         <v>3</v>
       </c>
-      <c r="G15" s="63">
+      <c r="H15" s="61">
         <v>2</v>
-      </c>
-      <c r="H15" s="63">
-        <v>1</v>
       </c>
       <c r="I15" s="31"/>
       <c r="J15" s="45"/>
       <c r="K15" s="29"/>
-      <c r="L15" s="63">
-        <v>2</v>
+      <c r="L15" s="61">
+        <v>3</v>
       </c>
       <c r="M15" s="30"/>
       <c r="N15" s="31"/>
       <c r="O15" s="45"/>
-      <c r="P15" s="62">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="63">
+      <c r="P15" s="60">
         <v>2</v>
       </c>
-      <c r="R15" s="63">
+      <c r="Q15" s="61">
         <v>3</v>
+      </c>
+      <c r="R15" s="61">
+        <v>4</v>
       </c>
       <c r="S15" s="31"/>
       <c r="T15" s="45"/>
       <c r="U15" s="29"/>
-      <c r="V15" s="63">
-        <v>2</v>
+      <c r="V15" s="61">
+        <v>3</v>
       </c>
       <c r="W15" s="30"/>
       <c r="X15" s="31"/>
@@ -13251,24 +13251,24 @@
       <c r="I16" s="31"/>
       <c r="J16" s="45"/>
       <c r="K16" s="29"/>
-      <c r="L16" s="63">
+      <c r="L16" s="61">
+        <v>2</v>
+      </c>
+      <c r="M16" s="61">
         <v>1</v>
-      </c>
-      <c r="M16" s="63">
-        <v>0</v>
       </c>
       <c r="N16" s="31"/>
       <c r="O16" s="45"/>
-      <c r="P16" s="62">
-        <v>0</v>
+      <c r="P16" s="60">
+        <v>1</v>
       </c>
       <c r="Q16" s="30"/>
       <c r="R16" s="30"/>
       <c r="S16" s="31"/>
       <c r="T16" s="45"/>
       <c r="U16" s="29"/>
-      <c r="V16" s="63">
-        <v>3</v>
+      <c r="V16" s="61">
+        <v>4</v>
       </c>
       <c r="W16" s="30"/>
       <c r="X16" s="31"/>
@@ -13570,38 +13570,38 @@
       <c r="D20" s="1"/>
       <c r="E20" s="45"/>
       <c r="F20" s="29"/>
-      <c r="G20" s="61">
-        <v>0</v>
-      </c>
-      <c r="H20" s="61">
+      <c r="G20" s="59">
         <v>1</v>
+      </c>
+      <c r="H20" s="59">
+        <v>2</v>
       </c>
       <c r="I20" s="31"/>
       <c r="J20" s="45"/>
       <c r="K20" s="29"/>
-      <c r="L20" s="61">
-        <v>3</v>
-      </c>
-      <c r="M20" s="61">
-        <v>0</v>
+      <c r="L20" s="59">
+        <v>4</v>
+      </c>
+      <c r="M20" s="59">
+        <v>1</v>
       </c>
       <c r="N20" s="31"/>
       <c r="O20" s="45"/>
       <c r="P20" s="29"/>
-      <c r="Q20" s="61">
-        <v>2</v>
-      </c>
-      <c r="R20" s="61">
+      <c r="Q20" s="59">
         <v>3</v>
+      </c>
+      <c r="R20" s="59">
+        <v>4</v>
       </c>
       <c r="S20" s="31"/>
       <c r="T20" s="45"/>
       <c r="U20" s="29"/>
-      <c r="V20" s="61">
-        <v>1</v>
-      </c>
-      <c r="W20" s="61">
+      <c r="V20" s="59">
         <v>2</v>
+      </c>
+      <c r="W20" s="59">
+        <v>3</v>
       </c>
       <c r="X20" s="31"/>
       <c r="Y20" s="45"/>
@@ -13665,38 +13665,38 @@
       <c r="D21" s="1"/>
       <c r="E21" s="45"/>
       <c r="F21" s="29"/>
-      <c r="G21" s="61">
+      <c r="G21" s="59">
+        <v>4</v>
+      </c>
+      <c r="H21" s="59">
         <v>3</v>
-      </c>
-      <c r="H21" s="61">
-        <v>2</v>
       </c>
       <c r="I21" s="31"/>
       <c r="J21" s="45"/>
       <c r="K21" s="29"/>
-      <c r="L21" s="61">
+      <c r="L21" s="59">
+        <v>3</v>
+      </c>
+      <c r="M21" s="59">
         <v>2</v>
-      </c>
-      <c r="M21" s="61">
-        <v>1</v>
       </c>
       <c r="N21" s="31"/>
       <c r="O21" s="45"/>
       <c r="P21" s="29"/>
-      <c r="Q21" s="61">
+      <c r="Q21" s="59">
+        <v>2</v>
+      </c>
+      <c r="R21" s="59">
         <v>1</v>
-      </c>
-      <c r="R21" s="61">
-        <v>0</v>
       </c>
       <c r="S21" s="31"/>
       <c r="T21" s="45"/>
       <c r="U21" s="29"/>
-      <c r="V21" s="61">
-        <v>0</v>
-      </c>
-      <c r="W21" s="61">
-        <v>3</v>
+      <c r="V21" s="59">
+        <v>1</v>
+      </c>
+      <c r="W21" s="59">
+        <v>4</v>
       </c>
       <c r="X21" s="31"/>
       <c r="Y21" s="45"/>
@@ -13918,17 +13918,17 @@
       <c r="D24" s="1"/>
       <c r="E24" s="45"/>
       <c r="F24" s="26"/>
-      <c r="G24" s="66">
+      <c r="G24" s="64">
+        <v>2</v>
+      </c>
+      <c r="H24" s="64">
         <v>1</v>
-      </c>
-      <c r="H24" s="66">
-        <v>0</v>
       </c>
       <c r="I24" s="28"/>
       <c r="J24" s="45"/>
       <c r="K24" s="26"/>
-      <c r="L24" s="66">
-        <v>3</v>
+      <c r="L24" s="64">
+        <v>4</v>
       </c>
       <c r="M24" s="27"/>
       <c r="N24" s="28"/>
@@ -13938,8 +13938,8 @@
       <c r="R24" s="27"/>
       <c r="S24" s="28"/>
       <c r="T24" s="45"/>
-      <c r="U24" s="69">
-        <v>0</v>
+      <c r="U24" s="67">
+        <v>1</v>
       </c>
       <c r="V24" s="27"/>
       <c r="W24" s="27"/>
@@ -14004,38 +14004,38 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="45"/>
-      <c r="F25" s="67">
+      <c r="F25" s="65">
+        <v>4</v>
+      </c>
+      <c r="G25" s="66">
         <v>3</v>
-      </c>
-      <c r="G25" s="68">
-        <v>2</v>
       </c>
       <c r="H25" s="30"/>
       <c r="I25" s="31"/>
       <c r="J25" s="45"/>
       <c r="K25" s="29"/>
-      <c r="L25" s="68">
+      <c r="L25" s="66">
+        <v>3</v>
+      </c>
+      <c r="M25" s="66">
         <v>2</v>
-      </c>
-      <c r="M25" s="68">
-        <v>1</v>
       </c>
       <c r="N25" s="31"/>
       <c r="O25" s="45"/>
       <c r="P25" s="29"/>
-      <c r="Q25" s="68">
-        <v>2</v>
-      </c>
-      <c r="R25" s="68">
+      <c r="Q25" s="66">
         <v>3</v>
+      </c>
+      <c r="R25" s="66">
+        <v>4</v>
       </c>
       <c r="S25" s="31"/>
       <c r="T25" s="45"/>
-      <c r="U25" s="67">
-        <v>1</v>
-      </c>
-      <c r="V25" s="68">
+      <c r="U25" s="65">
         <v>2</v>
+      </c>
+      <c r="V25" s="66">
+        <v>3</v>
       </c>
       <c r="W25" s="30"/>
       <c r="X25" s="31"/>
@@ -14106,23 +14106,23 @@
       <c r="J26" s="45"/>
       <c r="K26" s="29"/>
       <c r="L26" s="30"/>
-      <c r="M26" s="68">
-        <v>0</v>
+      <c r="M26" s="66">
+        <v>1</v>
       </c>
       <c r="N26" s="31"/>
       <c r="O26" s="45"/>
-      <c r="P26" s="67">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="68">
+      <c r="P26" s="65">
         <v>1</v>
+      </c>
+      <c r="Q26" s="66">
+        <v>2</v>
       </c>
       <c r="R26" s="30"/>
       <c r="S26" s="31"/>
       <c r="T26" s="45"/>
       <c r="U26" s="29"/>
-      <c r="V26" s="68">
-        <v>3</v>
+      <c r="V26" s="66">
+        <v>4</v>
       </c>
       <c r="W26" s="30"/>
       <c r="X26" s="31"/>
@@ -14345,15 +14345,15 @@
       <c r="D29" s="1"/>
       <c r="E29" s="45"/>
       <c r="F29" s="26"/>
-      <c r="G29" s="70">
-        <v>0</v>
+      <c r="G29" s="68">
+        <v>1</v>
       </c>
       <c r="H29" s="27"/>
       <c r="I29" s="28"/>
       <c r="J29" s="45"/>
       <c r="K29" s="26"/>
-      <c r="L29" s="70">
-        <v>1</v>
+      <c r="L29" s="68">
+        <v>2</v>
       </c>
       <c r="M29" s="27"/>
       <c r="N29" s="28"/>
@@ -14364,8 +14364,8 @@
       <c r="S29" s="28"/>
       <c r="T29" s="45"/>
       <c r="U29" s="26"/>
-      <c r="V29" s="70">
-        <v>3</v>
+      <c r="V29" s="68">
+        <v>4</v>
       </c>
       <c r="W29" s="27"/>
       <c r="X29" s="28"/>
@@ -14429,42 +14429,42 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="45"/>
-      <c r="F30" s="71">
-        <v>1</v>
-      </c>
-      <c r="G30" s="72">
+      <c r="F30" s="69">
         <v>2</v>
       </c>
-      <c r="H30" s="72">
+      <c r="G30" s="70">
         <v>3</v>
+      </c>
+      <c r="H30" s="70">
+        <v>4</v>
       </c>
       <c r="I30" s="31"/>
       <c r="J30" s="45"/>
       <c r="K30" s="29"/>
-      <c r="L30" s="72">
-        <v>2</v>
-      </c>
-      <c r="M30" s="72">
-        <v>0</v>
+      <c r="L30" s="70">
+        <v>3</v>
+      </c>
+      <c r="M30" s="70">
+        <v>1</v>
       </c>
       <c r="N30" s="31"/>
       <c r="O30" s="45"/>
-      <c r="P30" s="71">
+      <c r="P30" s="69">
+        <v>4</v>
+      </c>
+      <c r="Q30" s="70">
         <v>3</v>
       </c>
-      <c r="Q30" s="72">
+      <c r="R30" s="70">
         <v>2</v>
-      </c>
-      <c r="R30" s="72">
-        <v>1</v>
       </c>
       <c r="S30" s="31"/>
       <c r="T30" s="45"/>
-      <c r="U30" s="71">
-        <v>0</v>
-      </c>
-      <c r="V30" s="72">
-        <v>2</v>
+      <c r="U30" s="69">
+        <v>1</v>
+      </c>
+      <c r="V30" s="70">
+        <v>3</v>
       </c>
       <c r="W30" s="30"/>
       <c r="X30" s="31"/>
@@ -14534,22 +14534,22 @@
       <c r="I31" s="31"/>
       <c r="J31" s="45"/>
       <c r="K31" s="29"/>
-      <c r="L31" s="72">
-        <v>3</v>
+      <c r="L31" s="70">
+        <v>4</v>
       </c>
       <c r="M31" s="30"/>
       <c r="N31" s="31"/>
       <c r="O31" s="45"/>
       <c r="P31" s="29"/>
-      <c r="Q31" s="72">
-        <v>0</v>
+      <c r="Q31" s="70">
+        <v>1</v>
       </c>
       <c r="R31" s="30"/>
       <c r="S31" s="31"/>
       <c r="T31" s="45"/>
       <c r="U31" s="29"/>
-      <c r="V31" s="72">
-        <v>1</v>
+      <c r="V31" s="70">
+        <v>2</v>
       </c>
       <c r="W31" s="30"/>
       <c r="X31" s="31"/>
@@ -14771,19 +14771,19 @@
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="45"/>
-      <c r="F34" s="73">
-        <v>0</v>
-      </c>
-      <c r="G34" s="74">
+      <c r="F34" s="71">
         <v>1</v>
+      </c>
+      <c r="G34" s="72">
+        <v>2</v>
       </c>
       <c r="H34" s="27"/>
       <c r="I34" s="28"/>
       <c r="J34" s="45"/>
       <c r="K34" s="26"/>
       <c r="L34" s="27"/>
-      <c r="M34" s="74">
-        <v>0</v>
+      <c r="M34" s="72">
+        <v>1</v>
       </c>
       <c r="N34" s="28"/>
       <c r="O34" s="45"/>
@@ -14793,8 +14793,8 @@
       <c r="S34" s="28"/>
       <c r="T34" s="45"/>
       <c r="U34" s="26"/>
-      <c r="V34" s="74">
-        <v>3</v>
+      <c r="V34" s="72">
+        <v>4</v>
       </c>
       <c r="W34" s="27"/>
       <c r="X34" s="28"/>
@@ -14859,37 +14859,37 @@
       <c r="D35" s="1"/>
       <c r="E35" s="45"/>
       <c r="F35" s="29"/>
-      <c r="G35" s="75">
-        <v>2</v>
-      </c>
-      <c r="H35" s="75">
+      <c r="G35" s="73">
         <v>3</v>
+      </c>
+      <c r="H35" s="73">
+        <v>4</v>
       </c>
       <c r="I35" s="31"/>
       <c r="J35" s="45"/>
       <c r="K35" s="29"/>
-      <c r="L35" s="75">
+      <c r="L35" s="73">
+        <v>3</v>
+      </c>
+      <c r="M35" s="73">
         <v>2</v>
-      </c>
-      <c r="M35" s="75">
-        <v>1</v>
       </c>
       <c r="N35" s="31"/>
       <c r="O35" s="45"/>
-      <c r="P35" s="76">
+      <c r="P35" s="74">
+        <v>4</v>
+      </c>
+      <c r="Q35" s="73">
         <v>3</v>
-      </c>
-      <c r="Q35" s="75">
-        <v>2</v>
       </c>
       <c r="R35" s="30"/>
       <c r="S35" s="31"/>
       <c r="T35" s="45"/>
-      <c r="U35" s="76">
-        <v>1</v>
-      </c>
-      <c r="V35" s="75">
+      <c r="U35" s="74">
         <v>2</v>
+      </c>
+      <c r="V35" s="73">
+        <v>3</v>
       </c>
       <c r="W35" s="30"/>
       <c r="X35" s="31"/>
@@ -14959,23 +14959,23 @@
       <c r="I36" s="31"/>
       <c r="J36" s="45"/>
       <c r="K36" s="29"/>
-      <c r="L36" s="75">
-        <v>3</v>
+      <c r="L36" s="73">
+        <v>4</v>
       </c>
       <c r="M36" s="30"/>
       <c r="N36" s="31"/>
       <c r="O36" s="45"/>
       <c r="P36" s="29"/>
-      <c r="Q36" s="75">
+      <c r="Q36" s="73">
+        <v>2</v>
+      </c>
+      <c r="R36" s="73">
         <v>1</v>
-      </c>
-      <c r="R36" s="75">
-        <v>0</v>
       </c>
       <c r="S36" s="31"/>
       <c r="T36" s="45"/>
-      <c r="U36" s="76">
-        <v>0</v>
+      <c r="U36" s="74">
+        <v>1</v>
       </c>
       <c r="V36" s="30"/>
       <c r="W36" s="30"/>

</xml_diff>